<commit_message>
add StandardScaler results to spreadsheet, MinMax scaler seems better
</commit_message>
<xml_diff>
--- a/tuning_classifier_results.xlsx
+++ b/tuning_classifier_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="raw results 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="analysis 2" sheetId="5" r:id="rId4"/>
     <sheet name="analysis 3" sheetId="7" r:id="rId5"/>
     <sheet name="analysis 4" sheetId="8" r:id="rId6"/>
+    <sheet name="analysis 5" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="55">
   <si>
     <t>loss</t>
   </si>
@@ -139,15 +140,6 @@
     <t>avg f-score</t>
   </si>
   <si>
-    <t>50 iterations</t>
-  </si>
-  <si>
-    <t>200 iterations</t>
-  </si>
-  <si>
-    <t>500 iterations</t>
-  </si>
-  <si>
     <t>test_2018-06-27_21:53:46.log</t>
   </si>
   <si>
@@ -164,6 +156,45 @@
   </si>
   <si>
     <t>for comparison, the top 500 iteration results:</t>
+  </si>
+  <si>
+    <t>50 iterations, MinMax scaler</t>
+  </si>
+  <si>
+    <t>200 iterations, MinMax scaler</t>
+  </si>
+  <si>
+    <t>500 iterations, MinMax scaler</t>
+  </si>
+  <si>
+    <t>analysis of raw results 1</t>
+  </si>
+  <si>
+    <t>analysis for raw results 2</t>
+  </si>
+  <si>
+    <t>just analysis, no raw results (assuming I ever put these in)</t>
+  </si>
+  <si>
+    <t>just analysis, no raw results</t>
+  </si>
+  <si>
+    <t>50 iterations, StandardScaler</t>
+  </si>
+  <si>
+    <t>test_2018-06-29_13:46:35.log</t>
+  </si>
+  <si>
+    <t>test_2018-06-29_13:46:38.log</t>
+  </si>
+  <si>
+    <t>test_2018-06-29_13:46:40.log</t>
+  </si>
+  <si>
+    <t>test_2018-06-29_13:46:44.log</t>
+  </si>
+  <si>
+    <t>test_2018-06-29_13:46:46.log</t>
   </si>
 </sst>
 </file>
@@ -492,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K174" sqref="K174"/>
     </sheetView>
   </sheetViews>
@@ -3589,10 +3620,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:N181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3606,7 +3637,7 @@
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3629,10 +3660,10 @@
         <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3649,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3675,7 +3706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3707,7 +3738,7 @@
         <v>0.17264740674844459</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -3738,8 +3769,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>0.17219356404970904</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3775,7 +3809,7 @@
         <v>0.16996903520819479</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3807,7 +3841,7 @@
         <v>0.16618426812957721</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -3839,7 +3873,7 @@
         <v>0.12119806876144586</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -3871,7 +3905,7 @@
         <v>7.0410234382491624E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -3903,7 +3937,7 @@
         <v>5.9921633556847834E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3939,7 +3973,7 @@
         <v>5.9650672299334018E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3971,7 +4005,7 @@
         <v>5.2413056211970697E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -4003,7 +4037,7 @@
         <v>4.8061970996316469E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -4035,7 +4069,7 @@
         <v>4.7723219459120642E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -4067,7 +4101,7 @@
         <v>4.7637511019023603E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -7398,8 +7432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9524,10 +9558,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9542,7 +9576,7 @@
     <col min="15" max="15" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -9577,10 +9611,10 @@
         <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -9606,7 +9640,7 @@
         <v>0.50028531107684104</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -9650,7 +9684,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -9703,7 +9737,7 @@
         <v>0.7341847707300766</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -9756,7 +9790,7 @@
         <v>0.72543038306802354</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -9816,8 +9850,11 @@
         <f t="shared" ca="1" si="5"/>
         <v>0.72538551513064098</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -9870,7 +9907,7 @@
         <v>0.66973673379269483</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -9923,7 +9960,7 @@
         <v>0.60398718359564074</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -9976,7 +10013,7 @@
         <v>0.60120294679132535</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -10029,7 +10066,7 @@
         <v>0.59798139447675458</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -10090,7 +10127,7 @@
         <v>0.59755781262455765</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -10143,7 +10180,7 @@
         <v>0.53989999602787098</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -10196,7 +10233,7 @@
         <v>0.53989999602787098</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -10249,7 +10286,7 @@
         <v>0.52718829661718003</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -10302,7 +10339,7 @@
         <v>0.52699359565741999</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -10582,7 +10619,7 @@
         <v>0.50271100758165399</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -12306,10 +12343,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F81"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12324,7 +12361,7 @@
     <col min="15" max="15" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -12359,10 +12396,13 @@
         <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
       <c r="B2">
         <v>0</v>
       </c>
@@ -12379,7 +12419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -12414,7 +12454,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -12458,7 +12498,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -12502,7 +12542,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -12554,7 +12594,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -12598,7 +12638,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -12641,8 +12681,11 @@
         <f t="shared" ca="1" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -12686,7 +12729,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -12730,7 +12773,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -12782,7 +12825,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
@@ -12826,7 +12869,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
@@ -12870,7 +12913,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -12914,7 +12957,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
@@ -12958,7 +13001,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
@@ -14308,10 +14351,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S81"/>
+  <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14326,7 +14369,7 @@
     <col min="16" max="16" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -14361,12 +14404,12 @@
         <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -14390,9 +14433,9 @@
         <v>0.61980470418151301</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -14434,9 +14477,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -14463,33 +14506,33 @@
         <v>56</v>
       </c>
       <c r="N4" t="str">
-        <f ca="1">INDIRECT("C"&amp;M4)</f>
+        <f t="shared" ref="N4:N19" ca="1" si="0">INDIRECT("C"&amp;M4)</f>
         <v>l2</v>
       </c>
       <c r="O4" t="b">
-        <f ca="1">INDIRECT("D"&amp;M4)</f>
+        <f t="shared" ref="O4:O19" ca="1" si="1">INDIRECT("D"&amp;M4)</f>
         <v>0</v>
       </c>
       <c r="P4" t="str">
-        <f ca="1">INDIRECT("E"&amp;M4)</f>
+        <f t="shared" ref="P4:P19" ca="1" si="2">INDIRECT("E"&amp;M4)</f>
         <v>squared_hinge</v>
       </c>
       <c r="Q4" t="b">
-        <f ca="1">INDIRECT("F"&amp;M4)</f>
+        <f t="shared" ref="Q4:Q19" ca="1" si="3">INDIRECT("F"&amp;M4)</f>
         <v>1</v>
       </c>
       <c r="R4">
-        <f ca="1">INDIRECT("J"&amp;M4)</f>
+        <f t="shared" ref="R4:R19" ca="1" si="4">INDIRECT("J"&amp;M4)</f>
         <v>0.31051625336004363</v>
       </c>
       <c r="S4">
-        <f ca="1">INDIRECT("K"&amp;M4)</f>
+        <f t="shared" ref="S4:S19" ca="1" si="5">INDIRECT("K"&amp;M4)</f>
         <v>0.73640560188951143</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -14516,33 +14559,33 @@
         <v>46</v>
       </c>
       <c r="N5" t="str">
-        <f ca="1">INDIRECT("C"&amp;M5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>none</v>
       </c>
       <c r="O5" t="b">
-        <f ca="1">INDIRECT("D"&amp;M5)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P5" t="str">
-        <f ca="1">INDIRECT("E"&amp;M5)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q5" t="b">
-        <f ca="1">INDIRECT("F"&amp;M5)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R5">
-        <f ca="1">INDIRECT("J"&amp;M5)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.26330124271914279</v>
       </c>
       <c r="S5">
-        <f ca="1">INDIRECT("K"&amp;M5)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.68762268373731061</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -14577,33 +14620,36 @@
         <v>76</v>
       </c>
       <c r="N6" t="str">
-        <f ca="1">INDIRECT("C"&amp;M6)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>elasticnet</v>
       </c>
       <c r="O6" t="b">
-        <f ca="1">INDIRECT("D"&amp;M6)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P6" t="str">
-        <f ca="1">INDIRECT("E"&amp;M6)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q6" t="b">
-        <f ca="1">INDIRECT("F"&amp;M6)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R6">
-        <f ca="1">INDIRECT("J"&amp;M6)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.24599608460670197</v>
       </c>
       <c r="S6">
-        <f ca="1">INDIRECT("K"&amp;M6)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.67947742185723148</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -14630,33 +14676,33 @@
         <v>31</v>
       </c>
       <c r="N7" t="str">
-        <f ca="1">INDIRECT("C"&amp;M7)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l1</v>
       </c>
       <c r="O7" t="b">
-        <f ca="1">INDIRECT("D"&amp;M7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P7" t="str">
-        <f ca="1">INDIRECT("E"&amp;M7)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q7" t="b">
-        <f ca="1">INDIRECT("F"&amp;M7)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R7">
-        <f ca="1">INDIRECT("J"&amp;M7)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.2097258355013</v>
       </c>
       <c r="S7">
-        <f ca="1">INDIRECT("K"&amp;M7)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.67472174650220396</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -14683,33 +14729,33 @@
         <v>11</v>
       </c>
       <c r="N8" t="str">
-        <f ca="1">INDIRECT("C"&amp;M8)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>none</v>
       </c>
       <c r="O8" t="b">
-        <f ca="1">INDIRECT("D"&amp;M8)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P8" t="str">
-        <f ca="1">INDIRECT("E"&amp;M8)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q8" t="b">
-        <f ca="1">INDIRECT("F"&amp;M8)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R8">
-        <f ca="1">INDIRECT("J"&amp;M8)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.2097258355013</v>
       </c>
       <c r="S8">
-        <f ca="1">INDIRECT("K"&amp;M8)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.67472174650220396</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -14736,33 +14782,33 @@
         <v>66</v>
       </c>
       <c r="N9" t="str">
-        <f ca="1">INDIRECT("C"&amp;M9)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l1</v>
       </c>
       <c r="O9" t="b">
-        <f ca="1">INDIRECT("D"&amp;M9)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P9" t="str">
-        <f ca="1">INDIRECT("E"&amp;M9)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q9" t="b">
-        <f ca="1">INDIRECT("F"&amp;M9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R9">
-        <f ca="1">INDIRECT("J"&amp;M9)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.24405500722911699</v>
       </c>
       <c r="S9">
-        <f ca="1">INDIRECT("K"&amp;M9)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.67274312291987215</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -14789,33 +14835,33 @@
         <v>6</v>
       </c>
       <c r="N10" t="str">
-        <f ca="1">INDIRECT("C"&amp;M10)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>none</v>
       </c>
       <c r="O10" t="b">
-        <f ca="1">INDIRECT("D"&amp;M10)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P10" t="str">
-        <f ca="1">INDIRECT("E"&amp;M10)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q10" t="b">
-        <f ca="1">INDIRECT("F"&amp;M10)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R10">
-        <f ca="1">INDIRECT("J"&amp;M10)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.18902927502985462</v>
       </c>
       <c r="S10">
-        <f ca="1">INDIRECT("K"&amp;M10)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.60781649916756797</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -14850,33 +14896,33 @@
         <v>36</v>
       </c>
       <c r="N11" t="str">
-        <f ca="1">INDIRECT("C"&amp;M11)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>elasticnet</v>
       </c>
       <c r="O11" t="b">
-        <f ca="1">INDIRECT("D"&amp;M11)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P11" t="str">
-        <f ca="1">INDIRECT("E"&amp;M11)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q11" t="b">
-        <f ca="1">INDIRECT("F"&amp;M11)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R11">
-        <f ca="1">INDIRECT("J"&amp;M11)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.17851826482106342</v>
       </c>
       <c r="S11">
-        <f ca="1">INDIRECT("K"&amp;M11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.60330770725232763</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -14903,33 +14949,33 @@
         <v>26</v>
       </c>
       <c r="N12" t="str">
-        <f ca="1">INDIRECT("C"&amp;M12)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l1</v>
       </c>
       <c r="O12" t="b">
-        <f ca="1">INDIRECT("D"&amp;M12)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P12" t="str">
-        <f ca="1">INDIRECT("E"&amp;M12)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q12" t="b">
-        <f ca="1">INDIRECT("F"&amp;M12)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R12">
-        <f ca="1">INDIRECT("J"&amp;M12)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.17525544202020837</v>
       </c>
       <c r="S12">
-        <f ca="1">INDIRECT("K"&amp;M12)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.59939635639406297</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -14956,33 +15002,33 @@
         <v>16</v>
       </c>
       <c r="N13" t="str">
-        <f ca="1">INDIRECT("C"&amp;M13)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l2</v>
       </c>
       <c r="O13" t="b">
-        <f ca="1">INDIRECT("D"&amp;M13)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P13" t="str">
-        <f ca="1">INDIRECT("E"&amp;M13)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q13" t="b">
-        <f ca="1">INDIRECT("F"&amp;M13)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="R13">
-        <f ca="1">INDIRECT("J"&amp;M13)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.14938589466098828</v>
       </c>
       <c r="S13">
-        <f ca="1">INDIRECT("K"&amp;M13)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.58615074511621945</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -15009,33 +15055,33 @@
         <v>41</v>
       </c>
       <c r="N14" t="str">
-        <f ca="1">INDIRECT("C"&amp;M14)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>elasticnet</v>
       </c>
       <c r="O14" t="b">
-        <f ca="1">INDIRECT("D"&amp;M14)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P14" t="str">
-        <f ca="1">INDIRECT("E"&amp;M14)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q14" t="b">
-        <f ca="1">INDIRECT("F"&amp;M14)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f ca="1">INDIRECT("J"&amp;M14)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>6.80797643764183E-2</v>
       </c>
       <c r="S14">
-        <f ca="1">INDIRECT("K"&amp;M14)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.52597986910788797</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -15062,33 +15108,33 @@
         <v>21</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">INDIRECT("C"&amp;M15)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l2</v>
       </c>
       <c r="O15" t="b">
-        <f ca="1">INDIRECT("D"&amp;M15)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="P15" t="str">
-        <f ca="1">INDIRECT("E"&amp;M15)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q15" t="b">
-        <f ca="1">INDIRECT("F"&amp;M15)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f ca="1">INDIRECT("J"&amp;M15)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>4.0706375336725498E-2</v>
       </c>
       <c r="S15">
-        <f ca="1">INDIRECT("K"&amp;M15)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.50978933669467796</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -15123,33 +15169,33 @@
         <v>51</v>
       </c>
       <c r="N16" t="str">
-        <f ca="1">INDIRECT("C"&amp;M16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>none</v>
       </c>
       <c r="O16" t="b">
-        <f ca="1">INDIRECT("D"&amp;M16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" t="str">
-        <f ca="1">INDIRECT("E"&amp;M16)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q16" t="b">
-        <f ca="1">INDIRECT("F"&amp;M16)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R16">
-        <f ca="1">INDIRECT("J"&amp;M16)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1.7949348414064401E-2</v>
       </c>
       <c r="S16">
-        <f ca="1">INDIRECT("K"&amp;M16)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.50407495253240697</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -15176,33 +15222,33 @@
         <v>81</v>
       </c>
       <c r="N17" t="str">
-        <f ca="1">INDIRECT("C"&amp;M17)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>elasticnet</v>
       </c>
       <c r="O17" t="b">
-        <f ca="1">INDIRECT("D"&amp;M17)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P17" t="str">
-        <f ca="1">INDIRECT("E"&amp;M17)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q17" t="b">
-        <f ca="1">INDIRECT("F"&amp;M17)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R17">
-        <f ca="1">INDIRECT("J"&amp;M17)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1.30480167014613E-3</v>
       </c>
       <c r="S17">
-        <f ca="1">INDIRECT("K"&amp;M17)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.50027386478936198</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -15229,33 +15275,33 @@
         <v>61</v>
       </c>
       <c r="N18" t="str">
-        <f ca="1">INDIRECT("C"&amp;M18)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l2</v>
       </c>
       <c r="O18" t="b">
-        <f ca="1">INDIRECT("D"&amp;M18)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P18" t="str">
-        <f ca="1">INDIRECT("E"&amp;M18)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q18" t="b">
-        <f ca="1">INDIRECT("F"&amp;M18)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R18">
-        <f ca="1">INDIRECT("J"&amp;M18)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1.3024225058609E-3</v>
       </c>
       <c r="S18">
-        <f ca="1">INDIRECT("K"&amp;M18)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.50025097221440495</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -15282,33 +15328,33 @@
         <v>71</v>
       </c>
       <c r="N19" t="str">
-        <f ca="1">INDIRECT("C"&amp;M19)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>l1</v>
       </c>
       <c r="O19" t="b">
-        <f ca="1">INDIRECT("D"&amp;M19)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P19" t="str">
-        <f ca="1">INDIRECT("E"&amp;M19)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>squared_hinge</v>
       </c>
       <c r="Q19" t="b">
-        <f ca="1">INDIRECT("F"&amp;M19)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="R19">
-        <f ca="1">INDIRECT("J"&amp;M19)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>5.2308094677651297E-4</v>
       </c>
       <c r="S19">
-        <f ca="1">INDIRECT("K"&amp;M19)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.50010006184897704</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -15334,7 +15380,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -15368,7 +15414,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -15394,7 +15440,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -15420,7 +15466,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -15446,7 +15492,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -15472,7 +15518,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -15506,7 +15552,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -15532,7 +15578,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -15558,7 +15604,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -15584,7 +15630,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -15610,7 +15656,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -15644,7 +15690,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>6</v>
@@ -15670,7 +15716,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <v>6</v>
@@ -15696,7 +15742,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -15722,7 +15768,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35">
         <v>6</v>
@@ -15748,7 +15794,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>6</v>
@@ -15782,7 +15828,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>7</v>
@@ -15808,7 +15854,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>7</v>
@@ -15834,7 +15880,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>7</v>
@@ -15860,7 +15906,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>7</v>
@@ -15886,7 +15932,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>7</v>
@@ -15920,7 +15966,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B42">
         <v>8</v>
@@ -15946,7 +15992,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -15972,7 +16018,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44">
         <v>8</v>
@@ -15998,7 +16044,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B45">
         <v>8</v>
@@ -16024,7 +16070,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B46">
         <v>8</v>
@@ -16058,7 +16104,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>9</v>
@@ -16084,7 +16130,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B48">
         <v>9</v>
@@ -16110,7 +16156,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B49">
         <v>9</v>
@@ -16136,7 +16182,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B50">
         <v>9</v>
@@ -16162,7 +16208,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>9</v>
@@ -16196,7 +16242,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B52">
         <v>10</v>
@@ -16222,7 +16268,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B53">
         <v>10</v>
@@ -16248,7 +16294,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B54">
         <v>10</v>
@@ -16274,7 +16320,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B55">
         <v>10</v>
@@ -16300,7 +16346,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B56">
         <v>10</v>
@@ -16334,7 +16380,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B57">
         <v>11</v>
@@ -16360,7 +16406,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B58">
         <v>11</v>
@@ -16386,7 +16432,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B59">
         <v>11</v>
@@ -16412,7 +16458,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B60">
         <v>11</v>
@@ -16438,7 +16484,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B61">
         <v>11</v>
@@ -16472,7 +16518,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B62">
         <v>12</v>
@@ -16498,7 +16544,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B63">
         <v>12</v>
@@ -16524,7 +16570,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B64">
         <v>12</v>
@@ -16550,7 +16596,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B65">
         <v>12</v>
@@ -16576,7 +16622,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B66">
         <v>12</v>
@@ -16610,7 +16656,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B67">
         <v>13</v>
@@ -16636,7 +16682,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B68">
         <v>13</v>
@@ -16662,7 +16708,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B69">
         <v>13</v>
@@ -16688,7 +16734,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B70">
         <v>13</v>
@@ -16714,7 +16760,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B71">
         <v>13</v>
@@ -16748,7 +16794,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B72">
         <v>14</v>
@@ -16774,7 +16820,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B73">
         <v>14</v>
@@ -16800,7 +16846,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B74">
         <v>14</v>
@@ -16826,7 +16872,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B75">
         <v>14</v>
@@ -16852,7 +16898,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B76">
         <v>14</v>
@@ -16886,7 +16932,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B77">
         <v>15</v>
@@ -16912,7 +16958,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B78">
         <v>15</v>
@@ -16938,7 +16984,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B79">
         <v>15</v>
@@ -16964,7 +17010,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B80">
         <v>15</v>
@@ -16990,7 +17036,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B81">
         <v>15</v>
@@ -17029,4 +17075,1391 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="12" width="10.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>5.8770022629453703E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.54307509436670798</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>5.7877302840548102E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.539753286622771</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>5.8657165126377898E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.54261978119792997</v>
+      </c>
+      <c r="M4">
+        <v>26</v>
+      </c>
+      <c r="N4" t="str">
+        <f ca="1">INDIRECT("C"&amp;M4)</f>
+        <v>none</v>
+      </c>
+      <c r="O4" t="b">
+        <f ca="1">INDIRECT("D"&amp;M4)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" t="str">
+        <f ca="1">INDIRECT("E"&amp;M4)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q4" t="b">
+        <f ca="1">INDIRECT("F"&amp;M4)</f>
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <f ca="1">INDIRECT("J"&amp;M4)</f>
+        <v>7.9778737723081722E-2</v>
+      </c>
+      <c r="S4">
+        <f ca="1">INDIRECT("K"&amp;M4)</f>
+        <v>0.70589154855706937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>9.5256172985969403E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.61143549106183104</v>
+      </c>
+      <c r="M5">
+        <v>31</v>
+      </c>
+      <c r="N5" t="str">
+        <f ca="1">INDIRECT("C"&amp;M5)</f>
+        <v>l2</v>
+      </c>
+      <c r="O5" t="b">
+        <f ca="1">INDIRECT("D"&amp;M5)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" t="str">
+        <f ca="1">INDIRECT("E"&amp;M5)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q5" t="b">
+        <f ca="1">INDIRECT("F"&amp;M5)</f>
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <f ca="1">INDIRECT("J"&amp;M5)</f>
+        <v>7.8985710280231727E-2</v>
+      </c>
+      <c r="S5">
+        <f ca="1">INDIRECT("K"&amp;M5)</f>
+        <v>0.70263440858499648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.155051693829514</v>
+      </c>
+      <c r="H6">
+        <v>0.63244356007225</v>
+      </c>
+      <c r="J6">
+        <f>AVERAGE(G2:G6)</f>
+        <v>8.5122471482372619E-2</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.57386544266429795</v>
+      </c>
+      <c r="M6">
+        <v>41</v>
+      </c>
+      <c r="N6" t="str">
+        <f ca="1">INDIRECT("C"&amp;M6)</f>
+        <v>elasticnet</v>
+      </c>
+      <c r="O6" t="b">
+        <f ca="1">INDIRECT("D"&amp;M6)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" t="str">
+        <f ca="1">INDIRECT("E"&amp;M6)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q6" t="b">
+        <f ca="1">INDIRECT("F"&amp;M6)</f>
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <f ca="1">INDIRECT("J"&amp;M6)</f>
+        <v>7.7988112669397328E-2</v>
+      </c>
+      <c r="S6">
+        <f ca="1">INDIRECT("K"&amp;M6)</f>
+        <v>0.69908105656721842</v>
+      </c>
+      <c r="U6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.124401913875598</v>
+      </c>
+      <c r="H7">
+        <v>0.55076319784606698</v>
+      </c>
+      <c r="M7">
+        <v>36</v>
+      </c>
+      <c r="N7" t="str">
+        <f ca="1">INDIRECT("C"&amp;M7)</f>
+        <v>l1</v>
+      </c>
+      <c r="O7" t="b">
+        <f ca="1">INDIRECT("D"&amp;M7)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" t="str">
+        <f ca="1">INDIRECT("E"&amp;M7)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q7" t="b">
+        <f ca="1">INDIRECT("F"&amp;M7)</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f ca="1">INDIRECT("J"&amp;M7)</f>
+        <v>7.7046807819472776E-2</v>
+      </c>
+      <c r="S7">
+        <f ca="1">INDIRECT("K"&amp;M7)</f>
+        <v>0.69645204361744717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.124517068845398</v>
+      </c>
+      <c r="H8">
+        <v>0.55270994327547296</v>
+      </c>
+      <c r="M8">
+        <v>16</v>
+      </c>
+      <c r="N8" t="str">
+        <f ca="1">INDIRECT("C"&amp;M8)</f>
+        <v>l1</v>
+      </c>
+      <c r="O8" t="b">
+        <f ca="1">INDIRECT("D"&amp;M8)</f>
+        <v>1</v>
+      </c>
+      <c r="P8" t="str">
+        <f ca="1">INDIRECT("E"&amp;M8)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q8" t="b">
+        <f ca="1">INDIRECT("F"&amp;M8)</f>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f ca="1">INDIRECT("J"&amp;M8)</f>
+        <v>0.11564704869133054</v>
+      </c>
+      <c r="S8">
+        <f ca="1">INDIRECT("K"&amp;M8)</f>
+        <v>0.58751762036116673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.119076863404227</v>
+      </c>
+      <c r="H9">
+        <v>0.54906678007784304</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9" t="str">
+        <f ca="1">INDIRECT("C"&amp;M9)</f>
+        <v>none</v>
+      </c>
+      <c r="O9" t="b">
+        <f ca="1">INDIRECT("D"&amp;M9)</f>
+        <v>1</v>
+      </c>
+      <c r="P9" t="str">
+        <f ca="1">INDIRECT("E"&amp;M9)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q9" t="b">
+        <f ca="1">INDIRECT("F"&amp;M9)</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f ca="1">INDIRECT("J"&amp;M9)</f>
+        <v>8.5122471482372619E-2</v>
+      </c>
+      <c r="S9">
+        <f ca="1">INDIRECT("K"&amp;M9)</f>
+        <v>0.57386544266429795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.12422281436365901</v>
+      </c>
+      <c r="H10">
+        <v>0.55248529181863704</v>
+      </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
+      <c r="N10" t="str">
+        <f ca="1">INDIRECT("C"&amp;M10)</f>
+        <v>elasticnet</v>
+      </c>
+      <c r="O10" t="b">
+        <f ca="1">INDIRECT("D"&amp;M10)</f>
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f ca="1">INDIRECT("E"&amp;M10)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q10" t="b">
+        <f ca="1">INDIRECT("F"&amp;M10)</f>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f ca="1">INDIRECT("J"&amp;M10)</f>
+        <v>0.12420756860306778</v>
+      </c>
+      <c r="S10">
+        <f ca="1">INDIRECT("K"&amp;M10)</f>
+        <v>0.55264551702880915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.12336041973254799</v>
+      </c>
+      <c r="H11">
+        <v>0.551694765945133</v>
+      </c>
+      <c r="J11">
+        <f>AVERAGE(G7:G11)</f>
+        <v>0.12311581604428601</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(H7:H11)</f>
+        <v>0.5513439957926306</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11" t="str">
+        <f ca="1">INDIRECT("C"&amp;M11)</f>
+        <v>l2</v>
+      </c>
+      <c r="O11" t="b">
+        <f ca="1">INDIRECT("D"&amp;M11)</f>
+        <v>1</v>
+      </c>
+      <c r="P11" t="str">
+        <f ca="1">INDIRECT("E"&amp;M11)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q11" t="b">
+        <f ca="1">INDIRECT("F"&amp;M11)</f>
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <f ca="1">INDIRECT("J"&amp;M11)</f>
+        <v>0.12311581604428601</v>
+      </c>
+      <c r="S11">
+        <f ca="1">INDIRECT("K"&amp;M11)</f>
+        <v>0.5513439957926306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>5.9583949173854497E-2</v>
+      </c>
+      <c r="H12">
+        <v>0.545729028325732</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.13630654754852001</v>
+      </c>
+      <c r="H13">
+        <v>0.63673500915524595</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.13021158182603201</v>
+      </c>
+      <c r="H14">
+        <v>0.62668740088460995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>6.0675177172913701E-2</v>
+      </c>
+      <c r="H15">
+        <v>0.54714497967297804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.12850336924331501</v>
+      </c>
+      <c r="H16">
+        <v>0.57497069482806495</v>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(G13:G17)</f>
+        <v>0.11564704869133054</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE(H13:H17)</f>
+        <v>0.58751762036116673</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0.122538567665872</v>
+      </c>
+      <c r="H17">
+        <v>0.55205001726493497</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.124734504730642</v>
+      </c>
+      <c r="H18">
+        <v>0.55218120464480902</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.124710158551106</v>
+      </c>
+      <c r="H19">
+        <v>0.55324163664446602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.123929985946084</v>
+      </c>
+      <c r="H20">
+        <v>0.55205708848123303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.125124626121635</v>
+      </c>
+      <c r="H21">
+        <v>0.55369763810860295</v>
+      </c>
+      <c r="J21">
+        <f>AVERAGE(G17:G21)</f>
+        <v>0.12420756860306778</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE(H17:H21)</f>
+        <v>0.55264551702880915</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>7.6868202307596806E-2</v>
+      </c>
+      <c r="H22">
+        <v>0.69578149727385896</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>7.9576366861996595E-2</v>
+      </c>
+      <c r="H23">
+        <v>0.705659183217626</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>7.6322930800542699E-2</v>
+      </c>
+      <c r="H24">
+        <v>0.69327808772025001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>8.5045107564191494E-2</v>
+      </c>
+      <c r="H25">
+        <v>0.72383812372836398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>8.1081081081081002E-2</v>
+      </c>
+      <c r="H26">
+        <v>0.71090085084524801</v>
+      </c>
+      <c r="J26">
+        <f>AVERAGE(G22:G26)</f>
+        <v>7.9778737723081722E-2</v>
+      </c>
+      <c r="K26">
+        <f>AVERAGE(H22:H26)</f>
+        <v>0.70589154855706937</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>8.0774176674440396E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.71046345436915803</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>7.38162735392391E-2</v>
+      </c>
+      <c r="H28">
+        <v>0.68268024584808895</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>8.4901081630766304E-2</v>
+      </c>
+      <c r="H29">
+        <v>0.72318637363745297</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>7.9865815108702595E-2</v>
+      </c>
+      <c r="H30">
+        <v>0.707470322453844</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>7.5571204448010201E-2</v>
+      </c>
+      <c r="H31">
+        <v>0.68937164661643802</v>
+      </c>
+      <c r="J31">
+        <f>AVERAGE(G27:G31)</f>
+        <v>7.8985710280231727E-2</v>
+      </c>
+      <c r="K31">
+        <f>AVERAGE(H27:H31)</f>
+        <v>0.70263440858499648</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>8.2252497326766094E-2</v>
+      </c>
+      <c r="H32">
+        <v>0.71615890076008104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>7.5516236194274694E-2</v>
+      </c>
+      <c r="H33">
+        <v>0.68980775398608096</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>7.5706863188261503E-2</v>
+      </c>
+      <c r="H34">
+        <v>0.69136116542111703</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>7.6929428034759606E-2</v>
+      </c>
+      <c r="H35">
+        <v>0.69650234149761203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>7.4829014353301998E-2</v>
+      </c>
+      <c r="H36">
+        <v>0.688430056422345</v>
+      </c>
+      <c r="J36">
+        <f>AVERAGE(G32:G36)</f>
+        <v>7.7046807819472776E-2</v>
+      </c>
+      <c r="K36">
+        <f>AVERAGE(H32:H36)</f>
+        <v>0.69645204361744717</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>7.9704877715534903E-2</v>
+      </c>
+      <c r="H37">
+        <v>0.70329712765950203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>7.5779844801891094E-2</v>
+      </c>
+      <c r="H38">
+        <v>0.68974769517716505</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>7.3503132179957895E-2</v>
+      </c>
+      <c r="H39">
+        <v>0.68245789128217904</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>7.7727842425704394E-2</v>
+      </c>
+      <c r="H40">
+        <v>0.69867689081948003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>8.3224866223898297E-2</v>
+      </c>
+      <c r="H41">
+        <v>0.72122567789776604</v>
+      </c>
+      <c r="J41">
+        <f>AVERAGE(G37:G41)</f>
+        <v>7.7988112669397328E-2</v>
+      </c>
+      <c r="K41">
+        <f>AVERAGE(H37:H41)</f>
+        <v>0.69908105656721842</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="M4:S11">
+    <sortCondition descending="1" ref="S4:S11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added results for training on a single year
</commit_message>
<xml_diff>
--- a/tuning_classifier_results.xlsx
+++ b/tuning_classifier_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="raw results 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="analysis 5" sheetId="10" r:id="rId7"/>
     <sheet name="8-config template" sheetId="11" r:id="rId8"/>
     <sheet name="analysis 6" sheetId="12" r:id="rId9"/>
+    <sheet name="analysis 7" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2536" uniqueCount="65">
   <si>
     <t>loss</t>
   </si>
@@ -209,6 +210,24 @@
   </si>
   <si>
     <t>eh… enough of that, not very good</t>
+  </si>
+  <si>
+    <t>50 iterations, MinMax scaler, train 2014, predict Jan 2015</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_12:55:04.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_12:55:07.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_12:55:10.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_12:55:13.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_12:55:16.log</t>
   </si>
 </sst>
 </file>
@@ -3632,6 +3651,1414 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="12" width="10.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.35141268075639498</v>
+      </c>
+      <c r="H2">
+        <v>0.74109335857436298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0.33215757936339302</v>
+      </c>
+      <c r="H3">
+        <v>0.736611389765092</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.36053284708504202</v>
+      </c>
+      <c r="H4">
+        <v>0.71935254233336299</v>
+      </c>
+      <c r="M4">
+        <v>26</v>
+      </c>
+      <c r="N4" t="str">
+        <f ca="1">INDIRECT("C"&amp;M4)</f>
+        <v>none</v>
+      </c>
+      <c r="O4" t="b">
+        <f ca="1">INDIRECT("D"&amp;M4)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" t="str">
+        <f ca="1">INDIRECT("E"&amp;M4)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q4" t="b">
+        <f ca="1">INDIRECT("F"&amp;M4)</f>
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <f ca="1">INDIRECT("J"&amp;M4)</f>
+        <v>0.35905609616535183</v>
+      </c>
+      <c r="S4">
+        <f ca="1">INDIRECT("K"&amp;M4)</f>
+        <v>0.75163167717857005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.19173477076450399</v>
+      </c>
+      <c r="H5">
+        <v>0.59540747268744498</v>
+      </c>
+      <c r="M5">
+        <v>36</v>
+      </c>
+      <c r="N5" t="str">
+        <f ca="1">INDIRECT("C"&amp;M5)</f>
+        <v>l1</v>
+      </c>
+      <c r="O5" t="b">
+        <f ca="1">INDIRECT("D"&amp;M5)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" t="str">
+        <f ca="1">INDIRECT("E"&amp;M5)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q5" t="b">
+        <f ca="1">INDIRECT("F"&amp;M5)</f>
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <f ca="1">INDIRECT("J"&amp;M5)</f>
+        <v>0.36328031148956219</v>
+      </c>
+      <c r="S5">
+        <f ca="1">INDIRECT("K"&amp;M5)</f>
+        <v>0.75141802137945335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.36029138086882501</v>
+      </c>
+      <c r="H6">
+        <v>0.709391813661853</v>
+      </c>
+      <c r="J6">
+        <f>AVERAGE(G2:G6)</f>
+        <v>0.3192258517676318</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.70037131540442321</v>
+      </c>
+      <c r="M6">
+        <v>41</v>
+      </c>
+      <c r="N6" t="str">
+        <f ca="1">INDIRECT("C"&amp;M6)</f>
+        <v>elasticnet</v>
+      </c>
+      <c r="O6" t="b">
+        <f ca="1">INDIRECT("D"&amp;M6)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" t="str">
+        <f ca="1">INDIRECT("E"&amp;M6)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q6" t="b">
+        <f ca="1">INDIRECT("F"&amp;M6)</f>
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <f ca="1">INDIRECT("J"&amp;M6)</f>
+        <v>0.37153944606755318</v>
+      </c>
+      <c r="S6">
+        <f ca="1">INDIRECT("K"&amp;M6)</f>
+        <v>0.74804459431403258</v>
+      </c>
+      <c r="U6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.19487776484284</v>
+      </c>
+      <c r="H7">
+        <v>0.59687084822812997</v>
+      </c>
+      <c r="M7">
+        <v>31</v>
+      </c>
+      <c r="N7" t="str">
+        <f ca="1">INDIRECT("C"&amp;M7)</f>
+        <v>l2</v>
+      </c>
+      <c r="O7" t="b">
+        <f ca="1">INDIRECT("D"&amp;M7)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" t="str">
+        <f ca="1">INDIRECT("E"&amp;M7)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q7" t="b">
+        <f ca="1">INDIRECT("F"&amp;M7)</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f ca="1">INDIRECT("J"&amp;M7)</f>
+        <v>0.33373293223080341</v>
+      </c>
+      <c r="S7">
+        <f ca="1">INDIRECT("K"&amp;M7)</f>
+        <v>0.72016299883890844</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.18221600923843601</v>
+      </c>
+      <c r="H8">
+        <v>0.58629956469336797</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8" t="str">
+        <f ca="1">INDIRECT("C"&amp;M8)</f>
+        <v>none</v>
+      </c>
+      <c r="O8" t="b">
+        <f ca="1">INDIRECT("D"&amp;M8)</f>
+        <v>1</v>
+      </c>
+      <c r="P8" t="str">
+        <f ca="1">INDIRECT("E"&amp;M8)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q8" t="b">
+        <f ca="1">INDIRECT("F"&amp;M8)</f>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f ca="1">INDIRECT("J"&amp;M8)</f>
+        <v>0.3192258517676318</v>
+      </c>
+      <c r="S8">
+        <f ca="1">INDIRECT("K"&amp;M8)</f>
+        <v>0.70037131540442321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.19682700208583501</v>
+      </c>
+      <c r="H9">
+        <v>0.59123062156523798</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9" t="str">
+        <f ca="1">INDIRECT("C"&amp;M9)</f>
+        <v>l1</v>
+      </c>
+      <c r="O9" t="b">
+        <f ca="1">INDIRECT("D"&amp;M9)</f>
+        <v>1</v>
+      </c>
+      <c r="P9" t="str">
+        <f ca="1">INDIRECT("E"&amp;M9)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q9" t="b">
+        <f ca="1">INDIRECT("F"&amp;M9)</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f ca="1">INDIRECT("J"&amp;M9)</f>
+        <v>0.25046312857532083</v>
+      </c>
+      <c r="S9">
+        <f ca="1">INDIRECT("K"&amp;M9)</f>
+        <v>0.63940197561163559</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.19786910197869101</v>
+      </c>
+      <c r="H10">
+        <v>0.59810630194412795</v>
+      </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
+      <c r="N10" t="str">
+        <f ca="1">INDIRECT("C"&amp;M10)</f>
+        <v>elasticnet</v>
+      </c>
+      <c r="O10" t="b">
+        <f ca="1">INDIRECT("D"&amp;M10)</f>
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f ca="1">INDIRECT("E"&amp;M10)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q10" t="b">
+        <f ca="1">INDIRECT("F"&amp;M10)</f>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f ca="1">INDIRECT("J"&amp;M10)</f>
+        <v>0.1896396916808798</v>
+      </c>
+      <c r="S10">
+        <f ca="1">INDIRECT("K"&amp;M10)</f>
+        <v>0.59248265758150365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.188025790604851</v>
+      </c>
+      <c r="H11">
+        <v>0.58872468697545</v>
+      </c>
+      <c r="J11">
+        <f>AVERAGE(G7:G11)</f>
+        <v>0.1919631337501306</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(H7:H11)</f>
+        <v>0.59224640468126277</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11" t="str">
+        <f ca="1">INDIRECT("C"&amp;M11)</f>
+        <v>l2</v>
+      </c>
+      <c r="O11" t="b">
+        <f ca="1">INDIRECT("D"&amp;M11)</f>
+        <v>1</v>
+      </c>
+      <c r="P11" t="str">
+        <f ca="1">INDIRECT("E"&amp;M11)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q11" t="b">
+        <f ca="1">INDIRECT("F"&amp;M11)</f>
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <f ca="1">INDIRECT("J"&amp;M11)</f>
+        <v>0.1919631337501306</v>
+      </c>
+      <c r="S11">
+        <f ca="1">INDIRECT("K"&amp;M11)</f>
+        <v>0.59224640468126277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0.18952778670093101</v>
+      </c>
+      <c r="H12">
+        <v>0.586138799482252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.192194992008524</v>
+      </c>
+      <c r="H13">
+        <v>0.58488610407474495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.34883720930232498</v>
+      </c>
+      <c r="H14">
+        <v>0.71717147886415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0.185428136347663</v>
+      </c>
+      <c r="H15">
+        <v>0.59092894535496399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.33515555113805701</v>
+      </c>
+      <c r="H16">
+        <v>0.70616634110853704</v>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(G13:G17)</f>
+        <v>0.25046312857532083</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE(H13:H17)</f>
+        <v>0.63940197561163559</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0.19069975408003501</v>
+      </c>
+      <c r="H17">
+        <v>0.59785700865578195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.200497771603866</v>
+      </c>
+      <c r="H18">
+        <v>0.60060985601831995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.196175505910019</v>
+      </c>
+      <c r="H19">
+        <v>0.59255953935819805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.17268636750577601</v>
+      </c>
+      <c r="H20">
+        <v>0.58100218288005401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.18813905930470301</v>
+      </c>
+      <c r="H21">
+        <v>0.59038470099516405</v>
+      </c>
+      <c r="J21">
+        <f>AVERAGE(G17:G21)</f>
+        <v>0.1896396916808798</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE(H17:H21)</f>
+        <v>0.59248265758150365</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.38591804608119001</v>
+      </c>
+      <c r="H22">
+        <v>0.75001699081749995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.35962928473238398</v>
+      </c>
+      <c r="H23">
+        <v>0.74809232230088696</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.35249108025620002</v>
+      </c>
+      <c r="H24">
+        <v>0.74995208735272001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.35277882323422399</v>
+      </c>
+      <c r="H25">
+        <v>0.75681885977448904</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0.344463246522761</v>
+      </c>
+      <c r="H26">
+        <v>0.75327812564725405</v>
+      </c>
+      <c r="J26">
+        <f>AVERAGE(G22:G26)</f>
+        <v>0.35905609616535183</v>
+      </c>
+      <c r="K26">
+        <f>AVERAGE(H22:H26)</f>
+        <v>0.75163167717857005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0.34888644254382201</v>
+      </c>
+      <c r="H27">
+        <v>0.75071560417329697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0.35599043270276098</v>
+      </c>
+      <c r="H28">
+        <v>0.74991991415480797</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0.19076655052264799</v>
+      </c>
+      <c r="H29">
+        <v>0.61113237307648305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0.37376041715163599</v>
+      </c>
+      <c r="H30">
+        <v>0.74709002488505405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0.39926081823315002</v>
+      </c>
+      <c r="H31">
+        <v>0.74195707790489995</v>
+      </c>
+      <c r="J31">
+        <f>AVERAGE(G27:G31)</f>
+        <v>0.33373293223080341</v>
+      </c>
+      <c r="K31">
+        <f>AVERAGE(H27:H31)</f>
+        <v>0.72016299883890844</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0.37858366912139302</v>
+      </c>
+      <c r="H32">
+        <v>0.75181251025195495</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0.34279322202427798</v>
+      </c>
+      <c r="H33">
+        <v>0.75100934976297495</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0.36624464887512498</v>
+      </c>
+      <c r="H34">
+        <v>0.74677717427468904</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0.3843072247548</v>
+      </c>
+      <c r="H35">
+        <v>0.75738570766808</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0.34447279267221498</v>
+      </c>
+      <c r="H36">
+        <v>0.75010536493956803</v>
+      </c>
+      <c r="J36">
+        <f>AVERAGE(G32:G36)</f>
+        <v>0.36328031148956219</v>
+      </c>
+      <c r="K36">
+        <f>AVERAGE(H32:H36)</f>
+        <v>0.75141802137945335</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0.36303630363036299</v>
+      </c>
+      <c r="H37">
+        <v>0.74931126636286904</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0.359492288794868</v>
+      </c>
+      <c r="H38">
+        <v>0.74203554014496698</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0.387262846791877</v>
+      </c>
+      <c r="H39">
+        <v>0.75113486910562299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0.36419529837251302</v>
+      </c>
+      <c r="H40">
+        <v>0.74698267696870402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0.383710492748145</v>
+      </c>
+      <c r="H41">
+        <v>0.750758618988</v>
+      </c>
+      <c r="J41">
+        <f>AVERAGE(G37:G41)</f>
+        <v>0.37153944606755318</v>
+      </c>
+      <c r="K41">
+        <f>AVERAGE(H37:H41)</f>
+        <v>0.74804459431403258</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="M4:S11">
+    <sortCondition descending="1" ref="S4:S11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N181"/>
@@ -18482,7 +19909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
6-month training test results
</commit_message>
<xml_diff>
--- a/tuning_classifier_results.xlsx
+++ b/tuning_classifier_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="raw results 1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="analysis 6" sheetId="12" r:id="rId9"/>
     <sheet name="analysis 7" sheetId="13" r:id="rId10"/>
     <sheet name="analysis 8" sheetId="14" r:id="rId11"/>
+    <sheet name="analysis 9" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="77">
   <si>
     <t>loss</t>
   </si>
@@ -247,6 +248,24 @@
   </si>
   <si>
     <t>test_2018-07-05_15:53:57.log</t>
+  </si>
+  <si>
+    <t>50 iterations, MinMax scaler, train 2014 July-December, predict Jan 2015</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_16:00:04.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_16:00:02.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_16:00:00.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_16:00:07.log</t>
+  </si>
+  <si>
+    <t>test_2018-07-05_16:00:09.log</t>
   </si>
 </sst>
 </file>
@@ -5082,7 +5101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
@@ -6475,6 +6494,1414 @@
       <c r="K41">
         <f>AVERAGE(H37:H41)</f>
         <v>0.58880984553598881</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="M4:S11">
+    <sortCondition descending="1" ref="S4:S11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="12" width="10.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.190283881696163</v>
+      </c>
+      <c r="H2">
+        <v>0.59259165551979798</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0.30430320357745</v>
+      </c>
+      <c r="H3">
+        <v>0.74680750129720297</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.37163038777569501</v>
+      </c>
+      <c r="H4">
+        <v>0.73830387545846299</v>
+      </c>
+      <c r="M4">
+        <v>41</v>
+      </c>
+      <c r="N4" t="str">
+        <f ca="1">INDIRECT("C"&amp;M4)</f>
+        <v>elasticnet</v>
+      </c>
+      <c r="O4" t="b">
+        <f ca="1">INDIRECT("D"&amp;M4)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" t="str">
+        <f ca="1">INDIRECT("E"&amp;M4)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q4" t="b">
+        <f ca="1">INDIRECT("F"&amp;M4)</f>
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <f ca="1">INDIRECT("J"&amp;M4)</f>
+        <v>0.36335395445928242</v>
+      </c>
+      <c r="S4">
+        <f ca="1">INDIRECT("K"&amp;M4)</f>
+        <v>0.73828556482925367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.18825866254689899</v>
+      </c>
+      <c r="H5">
+        <v>0.59747764598506903</v>
+      </c>
+      <c r="M5">
+        <v>31</v>
+      </c>
+      <c r="N5" t="str">
+        <f ca="1">INDIRECT("C"&amp;M5)</f>
+        <v>l2</v>
+      </c>
+      <c r="O5" t="b">
+        <f ca="1">INDIRECT("D"&amp;M5)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" t="str">
+        <f ca="1">INDIRECT("E"&amp;M5)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q5" t="b">
+        <f ca="1">INDIRECT("F"&amp;M5)</f>
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <f ca="1">INDIRECT("J"&amp;M5)</f>
+        <v>0.32699974572268797</v>
+      </c>
+      <c r="S5">
+        <f ca="1">INDIRECT("K"&amp;M5)</f>
+        <v>0.71709155983945294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.20023188405797099</v>
+      </c>
+      <c r="H6">
+        <v>0.60031800420577697</v>
+      </c>
+      <c r="J6">
+        <f>AVERAGE(G2:G6)</f>
+        <v>0.25094160393083553</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.65509973649326203</v>
+      </c>
+      <c r="M6">
+        <v>16</v>
+      </c>
+      <c r="N6" t="str">
+        <f ca="1">INDIRECT("C"&amp;M6)</f>
+        <v>l1</v>
+      </c>
+      <c r="O6" t="b">
+        <f ca="1">INDIRECT("D"&amp;M6)</f>
+        <v>1</v>
+      </c>
+      <c r="P6" t="str">
+        <f ca="1">INDIRECT("E"&amp;M6)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q6" t="b">
+        <f ca="1">INDIRECT("F"&amp;M6)</f>
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <f ca="1">INDIRECT("J"&amp;M6)</f>
+        <v>0.34293534976242118</v>
+      </c>
+      <c r="S6">
+        <f ca="1">INDIRECT("K"&amp;M6)</f>
+        <v>0.6999791283116753</v>
+      </c>
+      <c r="U6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.17105094315411201</v>
+      </c>
+      <c r="H7">
+        <v>0.57656201010953101</v>
+      </c>
+      <c r="M7">
+        <v>36</v>
+      </c>
+      <c r="N7" t="str">
+        <f ca="1">INDIRECT("C"&amp;M7)</f>
+        <v>l1</v>
+      </c>
+      <c r="O7" t="b">
+        <f ca="1">INDIRECT("D"&amp;M7)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" t="str">
+        <f ca="1">INDIRECT("E"&amp;M7)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q7" t="b">
+        <f ca="1">INDIRECT("F"&amp;M7)</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f ca="1">INDIRECT("J"&amp;M7)</f>
+        <v>0.3029895180392394</v>
+      </c>
+      <c r="S7">
+        <f ca="1">INDIRECT("K"&amp;M7)</f>
+        <v>0.6924013908702068</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.17032714875762101</v>
+      </c>
+      <c r="H8">
+        <v>0.57482171426270601</v>
+      </c>
+      <c r="M8">
+        <v>26</v>
+      </c>
+      <c r="N8" t="str">
+        <f ca="1">INDIRECT("C"&amp;M8)</f>
+        <v>none</v>
+      </c>
+      <c r="O8" t="b">
+        <f ca="1">INDIRECT("D"&amp;M8)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" t="str">
+        <f ca="1">INDIRECT("E"&amp;M8)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q8" t="b">
+        <f ca="1">INDIRECT("F"&amp;M8)</f>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f ca="1">INDIRECT("J"&amp;M8)</f>
+        <v>0.26359501731898782</v>
+      </c>
+      <c r="S8">
+        <f ca="1">INDIRECT("K"&amp;M8)</f>
+        <v>0.6824808242542838</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.18333124765361</v>
+      </c>
+      <c r="H9">
+        <v>0.584784924228261</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9" t="str">
+        <f ca="1">INDIRECT("C"&amp;M9)</f>
+        <v>none</v>
+      </c>
+      <c r="O9" t="b">
+        <f ca="1">INDIRECT("D"&amp;M9)</f>
+        <v>1</v>
+      </c>
+      <c r="P9" t="str">
+        <f ca="1">INDIRECT("E"&amp;M9)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q9" t="b">
+        <f ca="1">INDIRECT("F"&amp;M9)</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f ca="1">INDIRECT("J"&amp;M9)</f>
+        <v>0.25094160393083553</v>
+      </c>
+      <c r="S9">
+        <f ca="1">INDIRECT("K"&amp;M9)</f>
+        <v>0.65509973649326203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.17318870977407499</v>
+      </c>
+      <c r="H10">
+        <v>0.58228811244666701</v>
+      </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
+      <c r="N10" t="str">
+        <f ca="1">INDIRECT("C"&amp;M10)</f>
+        <v>elasticnet</v>
+      </c>
+      <c r="O10" t="b">
+        <f ca="1">INDIRECT("D"&amp;M10)</f>
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f ca="1">INDIRECT("E"&amp;M10)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q10" t="b">
+        <f ca="1">INDIRECT("F"&amp;M10)</f>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f ca="1">INDIRECT("J"&amp;M10)</f>
+        <v>0.26950592772286541</v>
+      </c>
+      <c r="S10">
+        <f ca="1">INDIRECT("K"&amp;M10)</f>
+        <v>0.64065674919939497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.18046292663789701</v>
+      </c>
+      <c r="H11">
+        <v>0.58019790053396603</v>
+      </c>
+      <c r="J11">
+        <f>AVERAGE(G7:G11)</f>
+        <v>0.17567219519546301</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(H7:H11)</f>
+        <v>0.5797309323162263</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11" t="str">
+        <f ca="1">INDIRECT("C"&amp;M11)</f>
+        <v>l2</v>
+      </c>
+      <c r="O11" t="b">
+        <f ca="1">INDIRECT("D"&amp;M11)</f>
+        <v>1</v>
+      </c>
+      <c r="P11" t="str">
+        <f ca="1">INDIRECT("E"&amp;M11)</f>
+        <v>squared_hinge</v>
+      </c>
+      <c r="Q11" t="b">
+        <f ca="1">INDIRECT("F"&amp;M11)</f>
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <f ca="1">INDIRECT("J"&amp;M11)</f>
+        <v>0.17567219519546301</v>
+      </c>
+      <c r="S11">
+        <f ca="1">INDIRECT("K"&amp;M11)</f>
+        <v>0.5797309323162263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0.39655769325881601</v>
+      </c>
+      <c r="H12">
+        <v>0.74881435485263803</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.40152646424423399</v>
+      </c>
+      <c r="H13">
+        <v>0.72684144327266698</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.26875438186492101</v>
+      </c>
+      <c r="H14">
+        <v>0.70232942769931395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0.42026117926394901</v>
+      </c>
+      <c r="H15">
+        <v>0.73332886631790095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.22001462701121399</v>
+      </c>
+      <c r="H16">
+        <v>0.60693645681612396</v>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(G13:G17)</f>
+        <v>0.34293534976242118</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE(H13:H17)</f>
+        <v>0.6999791283116753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0.40412009642778801</v>
+      </c>
+      <c r="H17">
+        <v>0.73045944745237101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.18742496050552901</v>
+      </c>
+      <c r="H18">
+        <v>0.586251254507275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.16857413847613001</v>
+      </c>
+      <c r="H19">
+        <v>0.57618755299059399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.40471620510008199</v>
+      </c>
+      <c r="H20">
+        <v>0.73062164629051596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.18269423810479801</v>
+      </c>
+      <c r="H21">
+        <v>0.579763844756219</v>
+      </c>
+      <c r="J21">
+        <f>AVERAGE(G17:G21)</f>
+        <v>0.26950592772286541</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE(H17:H21)</f>
+        <v>0.64065674919939497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.172818554659878</v>
+      </c>
+      <c r="H22">
+        <v>0.60096100801392904</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.31840605759302398</v>
+      </c>
+      <c r="H23">
+        <v>0.74946656895325503</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.34355774301283099</v>
+      </c>
+      <c r="H24">
+        <v>0.73794585766305099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.33592806893393801</v>
+      </c>
+      <c r="H25">
+        <v>0.74434132444844403</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0.147264662395268</v>
+      </c>
+      <c r="H26">
+        <v>0.57968936219274003</v>
+      </c>
+      <c r="J26">
+        <f>AVERAGE(G22:G26)</f>
+        <v>0.26359501731898782</v>
+      </c>
+      <c r="K26">
+        <f>AVERAGE(H22:H26)</f>
+        <v>0.6824808242542838</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0.37981164853250399</v>
+      </c>
+      <c r="H27">
+        <v>0.75585217703336005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0.16673455532925999</v>
+      </c>
+      <c r="H28">
+        <v>0.60012357899300495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0.37955801104972298</v>
+      </c>
+      <c r="H29">
+        <v>0.753953583975286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0.34115725217092202</v>
+      </c>
+      <c r="H30">
+        <v>0.74108327558342302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0.36773726153103098</v>
+      </c>
+      <c r="H31">
+        <v>0.73444518361219102</v>
+      </c>
+      <c r="J31">
+        <f>AVERAGE(G27:G31)</f>
+        <v>0.32699974572268797</v>
+      </c>
+      <c r="K31">
+        <f>AVERAGE(H27:H31)</f>
+        <v>0.71709155983945294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0.35774332150196098</v>
+      </c>
+      <c r="H32">
+        <v>0.73483471675811396</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0.21478648820905</v>
+      </c>
+      <c r="H33">
+        <v>0.61756178890469704</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0.19497282608695601</v>
+      </c>
+      <c r="H34">
+        <v>0.61377755689314695</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0.39149175412293802</v>
+      </c>
+      <c r="H35">
+        <v>0.75833163305081797</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0.35595320027529198</v>
+      </c>
+      <c r="H36">
+        <v>0.73750125874425798</v>
+      </c>
+      <c r="J36">
+        <f>AVERAGE(G32:G36)</f>
+        <v>0.3029895180392394</v>
+      </c>
+      <c r="K36">
+        <f>AVERAGE(H32:H36)</f>
+        <v>0.6924013908702068</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0.41267486222975802</v>
+      </c>
+      <c r="H37">
+        <v>0.74328890669405301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0.37058327964715798</v>
+      </c>
+      <c r="H38">
+        <v>0.73073566616897301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0.326133174589676</v>
+      </c>
+      <c r="H39">
+        <v>0.73172702118956801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0.34925026776151302</v>
+      </c>
+      <c r="H40">
+        <v>0.73878370309194596</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0.35812818806830699</v>
+      </c>
+      <c r="H41">
+        <v>0.74689252700172803</v>
+      </c>
+      <c r="J41">
+        <f>AVERAGE(G37:G41)</f>
+        <v>0.36335395445928242</v>
+      </c>
+      <c r="K41">
+        <f>AVERAGE(H37:H41)</f>
+        <v>0.73828556482925367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plot comparing different training data ranges
</commit_message>
<xml_diff>
--- a/tuning_classifier_results.xlsx
+++ b/tuning_classifier_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="raw results 1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="analysis 7" sheetId="13" r:id="rId10"/>
     <sheet name="analysis 8" sheetId="14" r:id="rId11"/>
     <sheet name="analysis 9" sheetId="15" r:id="rId12"/>
+    <sheet name="Sheet5" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2931" uniqueCount="98">
   <si>
     <t>loss</t>
   </si>
@@ -267,6 +268,69 @@
   <si>
     <t>test_2018-07-05_16:00:09.log</t>
   </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>one month</t>
+  </si>
+  <si>
+    <t>six months</t>
+  </si>
+  <si>
+    <t>one year</t>
+  </si>
+  <si>
+    <t>1993-2014</t>
+  </si>
+  <si>
+    <t>1993-2015</t>
+  </si>
+  <si>
+    <t>1993-2016</t>
+  </si>
+  <si>
+    <t>1993-2017</t>
+  </si>
+  <si>
+    <t>1993-2018</t>
+  </si>
+  <si>
+    <t>1993-2019</t>
+  </si>
+  <si>
+    <t>1993-2020</t>
+  </si>
+  <si>
+    <t>1993-2021</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>Config 1</t>
+  </si>
+  <si>
+    <t>Config 2</t>
+  </si>
+  <si>
+    <t>Config 3</t>
+  </si>
+  <si>
+    <t>Config 4</t>
+  </si>
+  <si>
+    <t>Config 5</t>
+  </si>
+  <si>
+    <t>Config 6</t>
+  </si>
+  <si>
+    <t>Config 7</t>
+  </si>
+  <si>
+    <t>Config 8</t>
+  </si>
 </sst>
 </file>
 
@@ -327,6 +391,1252 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Adoption Classifier: Average AUROC Score by Training Data Range</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Classify</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> all January 2015 Events</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one month</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Config 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Config 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Config 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Config 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Config 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Config 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Config 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Config 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.58880984553598881</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5852121301592198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59563185380073391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59625331426436956</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59209807415833604</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58839414901841303</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5908386265948089</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.62271901611471159</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EA71-4B95-9BC2-610A884D17E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>six months</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Config 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Config 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Config 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Config 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Config 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Config 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Config 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Config 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.73828556482925367</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64065674919939497</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6924013908702068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6999791283116753</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71709155983945294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5797309323162263</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6824808242542838</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65509973649326203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EA71-4B95-9BC2-610A884D17E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Config 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Config 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Config 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Config 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Config 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Config 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Config 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Config 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.74804459431403258</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59248265758150365</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75141802137945335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63940197561163559</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72016299883890844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59224640468126277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75163167717857005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.70037131540442321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EA71-4B95-9BC2-610A884D17E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1993-2014</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Config 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Config 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Config 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Config 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Config 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Config 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Config 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Config 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.66973673379269483</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59755781262455765</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7341847707300766</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60398718359564074</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72538551513064098</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59798139447675458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72543038306802354</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60120294679132535</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EA71-4B95-9BC2-610A884D17E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1858949055"/>
+        <c:axId val="1858949887"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1858949055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858949887"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858949887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858949055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3694,7 +5004,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="M3" sqref="M3:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5102,7 +6412,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="N4" sqref="N4:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6509,8 +7819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7910,6 +9220,1047 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0.14777961664380562</v>
+      </c>
+      <c r="T2">
+        <v>0.58880984553598881</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3">
+        <f>INDEX(T:T,B$1+1)</f>
+        <v>0.58880984553598881</v>
+      </c>
+      <c r="C3">
+        <v>0.5852121301592198</v>
+      </c>
+      <c r="D3">
+        <v>0.59563185380073391</v>
+      </c>
+      <c r="E3">
+        <v>0.59625331426436956</v>
+      </c>
+      <c r="F3">
+        <v>0.59209807415833604</v>
+      </c>
+      <c r="G3">
+        <v>0.58839414901841303</v>
+      </c>
+      <c r="H3">
+        <v>0.5908386265948089</v>
+      </c>
+      <c r="I3">
+        <v>0.62271901611471159</v>
+      </c>
+      <c r="M3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0.36335395445928242</v>
+      </c>
+      <c r="T3">
+        <v>0.73828556482925367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4">
+        <f>INDEX(T:T,B$1+2)</f>
+        <v>0.73828556482925367</v>
+      </c>
+      <c r="C4">
+        <v>0.64065674919939497</v>
+      </c>
+      <c r="D4">
+        <v>0.6924013908702068</v>
+      </c>
+      <c r="E4">
+        <v>0.6999791283116753</v>
+      </c>
+      <c r="F4">
+        <v>0.71709155983945294</v>
+      </c>
+      <c r="G4">
+        <v>0.5797309323162263</v>
+      </c>
+      <c r="H4">
+        <v>0.6824808242542838</v>
+      </c>
+      <c r="I4">
+        <v>0.65509973649326203</v>
+      </c>
+      <c r="M4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0.37153944606755318</v>
+      </c>
+      <c r="T4">
+        <v>0.74804459431403258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <f>INDEX(T:T,B$1+3)</f>
+        <v>0.74804459431403258</v>
+      </c>
+      <c r="C5">
+        <v>0.59248265758150365</v>
+      </c>
+      <c r="D5">
+        <v>0.75141802137945335</v>
+      </c>
+      <c r="E5">
+        <v>0.63940197561163559</v>
+      </c>
+      <c r="F5">
+        <v>0.72016299883890844</v>
+      </c>
+      <c r="G5">
+        <v>0.59224640468126277</v>
+      </c>
+      <c r="H5">
+        <v>0.75163167717857005</v>
+      </c>
+      <c r="I5">
+        <v>0.70037131540442321</v>
+      </c>
+      <c r="M5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>0.24867356703995522</v>
+      </c>
+      <c r="T5">
+        <v>0.66973673379269483</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6">
+        <f>INDEX(T:T,B$1+4)</f>
+        <v>0.66973673379269483</v>
+      </c>
+      <c r="C6">
+        <v>0.59755781262455765</v>
+      </c>
+      <c r="D6">
+        <v>0.7341847707300766</v>
+      </c>
+      <c r="E6">
+        <v>0.60398718359564074</v>
+      </c>
+      <c r="F6">
+        <v>0.72538551513064098</v>
+      </c>
+      <c r="G6">
+        <v>0.59798139447675458</v>
+      </c>
+      <c r="H6">
+        <v>0.72543038306802354</v>
+      </c>
+      <c r="I6">
+        <v>0.60120294679132535</v>
+      </c>
+      <c r="M6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0.1541547655554808</v>
+      </c>
+      <c r="T6">
+        <v>0.5852121301592198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0.26950592772286541</v>
+      </c>
+      <c r="T7">
+        <v>0.64065674919939497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0.1896396916808798</v>
+      </c>
+      <c r="T8">
+        <v>0.59248265758150365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0.16899494921166561</v>
+      </c>
+      <c r="T9">
+        <v>0.59755781262455765</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>0.17297975119082939</v>
+      </c>
+      <c r="T10">
+        <v>0.59563185380073391</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>0.3029895180392394</v>
+      </c>
+      <c r="T11">
+        <v>0.6924013908702068</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0.36328031148956219</v>
+      </c>
+      <c r="T12">
+        <v>0.75141802137945335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>0.31447770458490482</v>
+      </c>
+      <c r="T13">
+        <v>0.7341847707300766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>0.14923450852250941</v>
+      </c>
+      <c r="T14">
+        <v>0.59625331426436956</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>10</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0.34293534976242118</v>
+      </c>
+      <c r="T15">
+        <v>0.6999791283116753</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>80</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0.25046312857532083</v>
+      </c>
+      <c r="T16">
+        <v>0.63940197561163559</v>
+      </c>
+    </row>
+    <row r="17" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M17" t="s">
+        <v>84</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>10</v>
+      </c>
+      <c r="R17" t="b">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>0.18167265962667739</v>
+      </c>
+      <c r="T17">
+        <v>0.60398718359564074</v>
+      </c>
+    </row>
+    <row r="18" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>10</v>
+      </c>
+      <c r="R18" t="b">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>0.16203119921134659</v>
+      </c>
+      <c r="T18">
+        <v>0.59209807415833604</v>
+      </c>
+    </row>
+    <row r="19" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M19" t="s">
+        <v>79</v>
+      </c>
+      <c r="N19">
+        <v>5</v>
+      </c>
+      <c r="O19" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>10</v>
+      </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>0.32699974572268797</v>
+      </c>
+      <c r="T19">
+        <v>0.71709155983945294</v>
+      </c>
+    </row>
+    <row r="20" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
+        <v>80</v>
+      </c>
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>0.33373293223080341</v>
+      </c>
+      <c r="T20">
+        <v>0.72016299883890844</v>
+      </c>
+    </row>
+    <row r="21" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M21" t="s">
+        <v>85</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>10</v>
+      </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>0.29663643298182063</v>
+      </c>
+      <c r="T21">
+        <v>0.72538551513064098</v>
+      </c>
+    </row>
+    <row r="22" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M22" t="s">
+        <v>78</v>
+      </c>
+      <c r="N22">
+        <v>6</v>
+      </c>
+      <c r="O22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>10</v>
+      </c>
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>0.1720052498347418</v>
+      </c>
+      <c r="T22">
+        <v>0.58839414901841303</v>
+      </c>
+    </row>
+    <row r="23" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>79</v>
+      </c>
+      <c r="N23">
+        <v>6</v>
+      </c>
+      <c r="O23" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>10</v>
+      </c>
+      <c r="R23" t="b">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>0.17567219519546301</v>
+      </c>
+      <c r="T23">
+        <v>0.5797309323162263</v>
+      </c>
+    </row>
+    <row r="24" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>80</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24" t="s">
+        <v>5</v>
+      </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>10</v>
+      </c>
+      <c r="R24" t="b">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>0.1919631337501306</v>
+      </c>
+      <c r="T24">
+        <v>0.59224640468126277</v>
+      </c>
+    </row>
+    <row r="25" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>86</v>
+      </c>
+      <c r="N25">
+        <v>6</v>
+      </c>
+      <c r="O25" t="s">
+        <v>5</v>
+      </c>
+      <c r="P25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>10</v>
+      </c>
+      <c r="R25" t="b">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>0.16863868420138978</v>
+      </c>
+      <c r="T25">
+        <v>0.59798139447675458</v>
+      </c>
+    </row>
+    <row r="26" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M26" t="s">
+        <v>78</v>
+      </c>
+      <c r="N26">
+        <v>7</v>
+      </c>
+      <c r="O26" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>10</v>
+      </c>
+      <c r="R26" t="b">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>0.15776196172229359</v>
+      </c>
+      <c r="T26">
+        <v>0.5908386265948089</v>
+      </c>
+    </row>
+    <row r="27" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M27" t="s">
+        <v>79</v>
+      </c>
+      <c r="N27">
+        <v>7</v>
+      </c>
+      <c r="O27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>10</v>
+      </c>
+      <c r="R27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>0.26359501731898782</v>
+      </c>
+      <c r="T27">
+        <v>0.6824808242542838</v>
+      </c>
+    </row>
+    <row r="28" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>80</v>
+      </c>
+      <c r="N28">
+        <v>7</v>
+      </c>
+      <c r="O28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>10</v>
+      </c>
+      <c r="R28" t="b">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>0.35905609616535183</v>
+      </c>
+      <c r="T28">
+        <v>0.75163167717857005</v>
+      </c>
+    </row>
+    <row r="29" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>87</v>
+      </c>
+      <c r="N29">
+        <v>7</v>
+      </c>
+      <c r="O29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>10</v>
+      </c>
+      <c r="R29" t="b">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>0.2920290081776844</v>
+      </c>
+      <c r="T29">
+        <v>0.72543038306802354</v>
+      </c>
+    </row>
+    <row r="30" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>78</v>
+      </c>
+      <c r="N30">
+        <v>8</v>
+      </c>
+      <c r="O30" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>10</v>
+      </c>
+      <c r="R30" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>0.19177266976806662</v>
+      </c>
+      <c r="T30">
+        <v>0.62271901611471159</v>
+      </c>
+    </row>
+    <row r="31" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>79</v>
+      </c>
+      <c r="N31">
+        <v>8</v>
+      </c>
+      <c r="O31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>10</v>
+      </c>
+      <c r="R31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>0.25094160393083553</v>
+      </c>
+      <c r="T31">
+        <v>0.65509973649326203</v>
+      </c>
+    </row>
+    <row r="32" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>80</v>
+      </c>
+      <c r="N32">
+        <v>8</v>
+      </c>
+      <c r="O32" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>10</v>
+      </c>
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>0.3192258517676318</v>
+      </c>
+      <c r="T32">
+        <v>0.70037131540442321</v>
+      </c>
+    </row>
+    <row r="33" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>88</v>
+      </c>
+      <c r="N33">
+        <v>8</v>
+      </c>
+      <c r="O33" t="s">
+        <v>4</v>
+      </c>
+      <c r="P33" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>10</v>
+      </c>
+      <c r="R33" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>0.17118534221565299</v>
+      </c>
+      <c r="T33">
+        <v>0.60120294679132535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13855,8 +16206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>